<commit_message>
Update non-text binary and regular file
</commit_message>
<xml_diff>
--- a/Test.xlsx
+++ b/Test.xlsx
@@ -11,12 +11,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Test</t>
   </si>
   <si>
     <t>Test2</t>
+  </si>
+  <si>
+    <t>Test3</t>
   </si>
 </sst>
 </file>
@@ -281,6 +284,11 @@
         <v>1</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>